<commit_message>
Add further test cases and fixes
</commit_message>
<xml_diff>
--- a/tests/data/input/json_to_rows.xlsx
+++ b/tests/data/input/json_to_rows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hassansyyid/Workspace/hg-opensrc/gluestick/tests/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usyyid/work/gluestick/tests/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A35FEE-BCC2-3048-BE6C-7560DF957A42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A56850-692F-4441-8C80-ADBC0C50D70D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{AC717DE3-7D7C-A348-9C21-FAEA2678FCD4}"/>
+    <workbookView xWindow="19340" yWindow="3440" windowWidth="28800" windowHeight="16260" xr2:uid="{AC717DE3-7D7C-A348-9C21-FAEA2678FCD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Metadata</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Customer Name</t>
   </si>
@@ -36,19 +33,31 @@
     <t>Company 1</t>
   </si>
   <si>
-    <t>{ "Id": 1, "Bio": { "Name": "John Smith", "Birthday": "01-01-1960" } }</t>
-  </si>
-  <si>
     <t>Company 2</t>
   </si>
   <si>
-    <t>{
-	"Id": 2,
-	"Bio": {
-		"Name": "Jane Smith",
-		"Birthday": "12-01-1960"
-	}
-}</t>
+    <t>Line Detail</t>
+  </si>
+  <si>
+    <t>[ {"Id": "1", "Desc": "Bolts", "Amount": 101.15}, {"Id": "2", "Desc": "Smith", "Amount": 90.80} ]</t>
+  </si>
+  <si>
+    <t>[ {"Id": "1", "Desc": "Braces", "Amount": 51.15}, {"Id": "2", "Desc": "Wood", "Amount": 190.10} ]</t>
+  </si>
+  <si>
+    <t>Company 3</t>
+  </si>
+  <si>
+    <t>[{"Id": "1", "Desc": "Braces", "Amount": 51.15}]</t>
+  </si>
+  <si>
+    <t>Company 4</t>
+  </si>
+  <si>
+    <t>Company 5</t>
+  </si>
+  <si>
+    <t>{"Id": "1", "Desc": "Braces", "Amount": 51.15}</t>
   </si>
 </sst>
 </file>
@@ -98,10 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -417,40 +425,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E4AF89-0327-8645-B170-EF4874FF5DB5}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1640625" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>